<commit_message>
Modified the UI front panel and Added Database columns
</commit_message>
<xml_diff>
--- a/lvsrc/SMOs/Instrument.Element2/Private/E2_status decode.xlsx
+++ b/lvsrc/SMOs/Instrument.Element2/Private/E2_status decode.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\ansom\users\Pubudu\Element2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ansom\Documents\GitHub\Element-2-Monitor\lvsrc\SMOs\Instrument.Element2\Private\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84909FF1-2A30-4D87-BDC6-5BEC073CEE0B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BE3C45-77F6-4961-9866-EE608EF87978}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{75692F6C-5106-4157-AEBC-29EA1E43CA76}"/>
   </bookViews>
@@ -54,12 +54,6 @@
     <t>SS</t>
   </si>
   <si>
-    <t>Laser status</t>
-  </si>
-  <si>
-    <t>Pump Status</t>
-  </si>
-  <si>
     <t>Pico Speed</t>
   </si>
   <si>
@@ -174,7 +168,13 @@
     <t>Diode Current Actual</t>
   </si>
   <si>
-    <t>Power</t>
+    <t>Laser status 2</t>
+  </si>
+  <si>
+    <t>Laser status 1</t>
+  </si>
+  <si>
+    <t>Pump Power</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <dimension ref="A1:C144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,7 +635,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -648,7 +648,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -711,7 +711,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -719,7 +719,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -957,7 +957,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -965,7 +965,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -973,7 +973,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -981,7 +981,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -989,7 +989,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1022,7 +1022,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -1030,7 +1030,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -1066,7 +1066,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -1074,7 +1074,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -1082,7 +1082,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -1090,7 +1090,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -1098,7 +1098,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -1121,7 +1121,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -1129,7 +1129,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -1137,7 +1137,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -1145,7 +1145,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -1153,7 +1153,7 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -1171,10 +1171,10 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C108" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -1182,7 +1182,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -1190,7 +1190,7 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -1198,7 +1198,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -1206,10 +1206,10 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C112" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -1217,7 +1217,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -1225,7 +1225,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -1233,7 +1233,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -1241,7 +1241,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -1249,10 +1249,10 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C117" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -1260,7 +1260,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -1268,7 +1268,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -1276,7 +1276,7 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -1284,7 +1284,7 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -1292,7 +1292,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -1300,7 +1300,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -1308,7 +1308,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -1316,7 +1316,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -1374,7 +1374,7 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -1382,7 +1382,7 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -1415,7 +1415,7 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>